<commit_message>
Han 11 2021 updates (major)
LOADS of updates and improvements:
1. Updated viral load model of Xi, He Aug 2020 Narue Medicine
2. Parameters all changeable in Fixed U menu
3. Vax % for modelling 1 or 2 shot for % of susceptibles in the visible Universe - protection schedule hard coded in Javascript
4. Inflation factor for each visible Universe so that size is not hard coded to agents
5. Specific day schedule entries debugged - these are pint changes not continuing
6. Console log updated to reflect parameter changes as well as time that transition to symptomatic takes place
7. With console log, entire transmission trees and family and universe transmissions can be recreated
8. New code and index files have "Clover" associated.
9. New data files in /data with prefix "Full"....you may have to recreate the cvs files from the FullSummary Excel sheet....
10. The new version should be backwards compatible to all existing .csv files
</commit_message>
<xml_diff>
--- a/docs/Population.xlsx
+++ b/docs/Population.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-8" yWindow="14198" windowWidth="17295" windowHeight="14220" activeTab="1"/>
-    <workbookView xWindow="-8" yWindow="-8" windowWidth="17295" windowHeight="14205"/>
+    <workbookView xWindow="-8" yWindow="14198" windowWidth="17295" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -2732,9 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE763"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A493" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="K370" sqref="K370"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13161,7 +13159,7 @@
         <v>5</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H287" s="157">
         <v>5</v>
@@ -30190,13 +30188,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="3" max="3" width="14.59765625" customWidth="1"/>
+    <col min="4" max="4" width="12.73046875" customWidth="1"/>
     <col min="10" max="11" width="34.1328125" customWidth="1"/>
     <col min="12" max="12" width="34.1328125" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="34.1328125" customWidth="1"/>
@@ -30717,7 +30716,9 @@
       <c r="M24" s="82" t="s">
         <v>198</v>
       </c>
-      <c r="N24" s="82"/>
+      <c r="N24" s="82">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B25" s="79" t="s">
@@ -30750,7 +30751,9 @@
       <c r="M25" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="N25" s="82"/>
+      <c r="N25" s="82">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B26" s="79" t="s">
@@ -30783,7 +30786,9 @@
       <c r="M26" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="N26" s="82"/>
+      <c r="N26" s="82">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B27" s="79" t="s">
@@ -30816,7 +30821,9 @@
       <c r="M27" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="N27" s="82"/>
+      <c r="N27" s="82">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B28" s="79" t="s">
@@ -30851,7 +30858,9 @@
       <c r="M28" s="82" t="s">
         <v>220</v>
       </c>
-      <c r="N28" s="82"/>
+      <c r="N28" s="82">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B29" s="79" t="s">
@@ -30886,7 +30895,9 @@
       <c r="M29" s="82" t="s">
         <v>180</v>
       </c>
-      <c r="N29" s="82"/>
+      <c r="N29" s="82">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B30" s="79" t="s">
@@ -30913,7 +30924,9 @@
       <c r="M30" s="82" t="s">
         <v>180</v>
       </c>
-      <c r="N30" s="82"/>
+      <c r="N30" s="82">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B31" s="79" t="s">
@@ -30938,7 +30951,9 @@
       <c r="M31" s="82" t="s">
         <v>229</v>
       </c>
-      <c r="N31" s="82"/>
+      <c r="N31" s="82">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B32" s="79" t="s">
@@ -30963,7 +30978,9 @@
       <c r="M32" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="N32" s="82"/>
+      <c r="N32" s="82">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B33" s="79" t="s">
@@ -30988,7 +31005,9 @@
       <c r="M33" s="82" t="s">
         <v>232</v>
       </c>
-      <c r="N33" s="82"/>
+      <c r="N33" s="82">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B34" s="79" t="s">
@@ -31011,7 +31030,9 @@
       <c r="M34" s="82" t="s">
         <v>233</v>
       </c>
-      <c r="N34" s="82"/>
+      <c r="N34" s="82">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B35" s="79" t="s">
@@ -31034,7 +31055,9 @@
       <c r="M35" s="82" t="s">
         <v>234</v>
       </c>
-      <c r="N35" s="82"/>
+      <c r="N35" s="82">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B36" s="79" t="s">
@@ -31057,7 +31080,9 @@
       <c r="M36" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="N36" s="82"/>
+      <c r="N36" s="82">
+        <v>11</v>
+      </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B37" s="79" t="s">
@@ -31080,7 +31105,9 @@
       <c r="M37" s="82" t="s">
         <v>237</v>
       </c>
-      <c r="N37" s="82"/>
+      <c r="N37" s="82">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B38" s="79"/>
@@ -31095,7 +31122,10 @@
       <c r="K38" s="79"/>
       <c r="L38" s="79"/>
       <c r="M38" s="78"/>
-      <c r="N38" s="78"/>
+      <c r="N38" s="78">
+        <f>AVERAGE(N24:N37)</f>
+        <v>6.6428571428571432</v>
+      </c>
     </row>
     <row r="39" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B39" s="79" t="s">
@@ -32751,7 +32781,6 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -33358,7 +33387,6 @@
   <dimension ref="A1:BE750"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>